<commit_message>
Added SRS Version 1.5 including context diagram and modified all the requirements in the SRS Updated SRS_review Sheet Signed-off-by: MostafaNader96 <mnader96@gmail.com>
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/SRS_Review.xlsx
+++ b/Software Specification/SRS/SRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -185,25 +185,25 @@
     <t>All req of SRS need to be reconsidered as above methodolgy of writing the SRS</t>
   </si>
   <si>
-    <t>Added Status Table</t>
-  </si>
-  <si>
-    <t>Modified</t>
-  </si>
-  <si>
-    <t>Added reference table</t>
-  </si>
-  <si>
-    <t>Added sw context diagram</t>
-  </si>
-  <si>
-    <t>all requiremets are changed to atomic requirements</t>
-  </si>
-  <si>
-    <t>added this template for each requirement</t>
-  </si>
-  <si>
-    <t>updated and modified this requirement to sw wise level</t>
+    <t>Added status table as required</t>
+  </si>
+  <si>
+    <t>There was a misconcept but it is modified</t>
+  </si>
+  <si>
+    <t>Added reference document</t>
+  </si>
+  <si>
+    <t>Added SW Context diagram descirbing the whole sw signals</t>
+  </si>
+  <si>
+    <t>modified all the requirements to atomic requirements</t>
+  </si>
+  <si>
+    <t>modified the requirements to the required table template</t>
+  </si>
+  <si>
+    <t>modified this requirement to sw not system requirement</t>
   </si>
   <si>
     <t>modified</t>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -978,13 +978,13 @@
       <selection activeCell="E14" sqref="E14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
@@ -997,7 +997,7 @@
       <c r="G3" s="26"/>
       <c r="H3" s="29"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="27"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1006,7 +1006,7 @@
       <c r="G4" s="28"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="27"/>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -1015,7 +1015,7 @@
       <c r="G5" s="28"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="G6" s="31"/>
       <c r="H6" s="32"/>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1041,7 @@
       <c r="G7" s="31"/>
       <c r="H7" s="32"/>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="25" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1054,7 @@
       <c r="G8" s="31"/>
       <c r="H8" s="32"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
         <v>9</v>
       </c>
@@ -1067,7 +1067,7 @@
       <c r="G9" s="31"/>
       <c r="H9" s="32"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="38"/>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -1076,7 +1076,7 @@
       <c r="G10" s="39"/>
       <c r="H10" s="40"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
@@ -1087,7 +1087,7 @@
       <c r="G11" s="34"/>
       <c r="H11" s="35"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="H12" s="35"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="H13" s="32"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -1130,7 +1130,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="32"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -1139,7 +1139,7 @@
       <c r="G15" s="31"/>
       <c r="H15" s="32"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="31"/>
       <c r="D16" s="31"/>
@@ -1148,7 +1148,7 @@
       <c r="G16" s="31"/>
       <c r="H16" s="32"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -1157,7 +1157,7 @@
       <c r="G17" s="31"/>
       <c r="H17" s="32"/>
     </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="36"/>
       <c r="D18" s="36"/>
@@ -1211,24 +1211,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>41</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>41</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>41</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1549,7 +1549,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1560,7 +1560,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1571,7 +1571,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1582,7 +1582,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1593,7 +1593,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1604,7 +1604,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1615,7 +1615,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1626,7 +1626,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1637,7 +1637,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1648,7 +1648,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1659,7 +1659,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1670,7 +1670,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1681,7 +1681,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1692,7 +1692,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1703,7 +1703,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1714,7 +1714,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1725,7 +1725,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1736,7 +1736,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1747,7 +1747,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1758,7 +1758,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1769,7 +1769,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1780,7 +1780,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1791,7 +1791,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1802,7 +1802,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1813,7 +1813,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1824,7 +1824,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1835,7 +1835,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1846,7 +1846,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1857,7 +1857,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1868,7 +1868,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1879,7 +1879,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1890,7 +1890,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1901,7 +1901,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1912,7 +1912,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1923,7 +1923,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>

</xml_diff>

<commit_message>
Update SRS review sheet
</commit_message>
<xml_diff>
--- a/Software Specification/SRS/SRS_Review.xlsx
+++ b/Software Specification/SRS/SRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="51">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">Software requirement </t>
   </si>
   <si>
-    <t xml:space="preserve">The goal of the SW req is to descrip what in specific software shall do , so you shall keep the SRS req atmoic means do one thing , and try to make an input and out put for it as much as you can </t>
-  </si>
-  <si>
     <t xml:space="preserve">you could represent each req in a table for more organization this table as follows :
 Req ID : xxx
 Description : xxxxxx
@@ -185,34 +182,22 @@
     <t>All req of SRS need to be reconsidered as above methodolgy of writing the SRS</t>
   </si>
   <si>
-    <t>Added status table as required</t>
-  </si>
-  <si>
-    <t>There was a misconcept but it is modified</t>
-  </si>
-  <si>
-    <t>Added reference document</t>
-  </si>
-  <si>
-    <t>Added SW Context diagram descirbing the whole sw signals</t>
-  </si>
-  <si>
-    <t>modified all the requirements to atomic requirements</t>
-  </si>
-  <si>
-    <t>modified the requirements to the required table template</t>
-  </si>
-  <si>
-    <t>modified this requirement to sw not system requirement</t>
-  </si>
-  <si>
-    <t>modified</t>
+    <t>The goal of the SW req is to descrip what in specific software shall do , so you shall keep the SRS req atmoic means do one thing , and try to make an input and out put for it as much as you can ,also the SRS shall not mention variables as this is not yet the SW , the SRS shall describe in abstraction way.</t>
+  </si>
+  <si>
+    <t>V1.3</t>
+  </si>
+  <si>
+    <t>23/2/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upate the review sheet after looking at the req </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -580,12 +565,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -597,36 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -974,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,189 +970,214 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="29"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="30"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
+      <c r="D13" s="25"/>
+      <c r="E13" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="32"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1184,23 +1194,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1211,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,13 +1252,13 @@
     </row>
     <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>32</v>
@@ -1280,53 +1273,49 @@
         <v>20</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>49</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I3" s="10"/>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>32</v>
@@ -1341,24 +1330,22 @@
         <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I4" s="10"/>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>32</v>
@@ -1373,21 +1360,19 @@
         <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>32</v>
@@ -1396,30 +1381,28 @@
         <v>36</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>52</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I6" s="12"/>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>32</v>
@@ -1428,30 +1411,28 @@
         <v>36</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>53</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I7" s="12"/>
       <c r="K7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>32</v>
@@ -1460,27 +1441,25 @@
         <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>32</v>
@@ -1489,25 +1468,25 @@
         <v>36</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="12" t="s">
-        <v>54</v>
-      </c>
+      <c r="H9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>32</v>
@@ -1516,15 +1495,15 @@
         <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="H10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="12"/>
       <c r="K10" t="s">
         <v>23</v>
       </c>

</xml_diff>